<commit_message>
fix: renomeando tabela no excel
</commit_message>
<xml_diff>
--- a/python/dashboard_data.xlsx
+++ b/python/dashboard_data.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Arquivos" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ArquivoData" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TemplateInfo" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="TemplatesMes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -452,10 +452,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="C2" t="n">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -497,17 +497,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>quantidade</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D2" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
@@ -517,13 +517,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" t="n">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D3" t="n">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -548,7 +548,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>month</t>
+          <t>mes</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -604,10 +604,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -620,10 +620,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>